<commit_message>
Egg clutch/and new growth parameter
</commit_message>
<xml_diff>
--- a/Pomacea/Population/PopulationSize_RepDD.xlsx
+++ b/Pomacea/Population/PopulationSize_RepDD.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{20CDC804-FD46-4E39-93B6-9B1163B1E55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D88AF17-FC54-4E16-9EE1-33C64D0C9D88}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E5FB4C3-E5AC-46D6-8A4B-1AB06A41F2A8}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{7E5FB4C3-E5AC-46D6-8A4B-1AB06A41F2A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5FF4E0DB-FDEF-4E60-80D8-F228879123CA}" type="CELLRANGE">
+                    <a:fld id="{C89FCA22-24F8-425C-B1FC-098263079DDA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -305,7 +305,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C7DE97E-4C1D-49ED-95EF-79478D02A337}" type="CELLRANGE">
+                    <a:fld id="{97A909DD-F3C5-4FF3-BBF6-757E111C810F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -338,7 +338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AEB870A8-2E71-42C3-B7CB-DF86759EBC27}" type="CELLRANGE">
+                    <a:fld id="{842B720A-8C4C-4F8D-89DC-05873DCAEF82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -371,7 +371,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{204F4618-6DC3-4C46-9879-43FB14ADAAA8}" type="CELLRANGE">
+                    <a:fld id="{50DD3CEF-79B4-4417-AC7B-D93EE422ED52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -404,7 +404,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95853A02-FEC7-42FF-B18E-EA16D6E9E3E9}" type="CELLRANGE">
+                    <a:fld id="{75721890-7063-43A6-9C19-3E901F854263}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -437,7 +437,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7284CB16-3289-48C2-95E2-9F52ADC01457}" type="CELLRANGE">
+                    <a:fld id="{D4E86B37-B4E5-4D6A-A17E-B66947BF49AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -470,7 +470,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48B82DFC-A919-4A94-B9BE-F9EA0981804E}" type="CELLRANGE">
+                    <a:fld id="{C280EE53-9267-4EEB-BD04-3EE3338E9B57}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -503,7 +503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13712A4C-32AF-408E-9106-35A1F2CBA8EA}" type="CELLRANGE">
+                    <a:fld id="{596AED8E-09F5-4022-B3A6-586460296B3A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -536,7 +536,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77CCD24F-B4D1-4407-B75F-7498C9D9A13D}" type="CELLRANGE">
+                    <a:fld id="{0E8B73D9-FFC5-4A69-87B3-C459EA948254}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1172,7 +1172,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF52C0BE-36A6-42A2-8A9C-E2D8B6B53B27}" type="CELLRANGE">
+                    <a:fld id="{FCAA5372-1D48-4987-8868-DEDF99FE160F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1206,7 +1206,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAC266C1-8E29-4771-963A-E87B8646BA70}" type="CELLRANGE">
+                    <a:fld id="{6E6C6BEC-EDEE-4CAF-BAA0-AEA1FDFD709A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1240,7 +1240,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A14665BC-E65C-45E9-9D06-55A8169A61CF}" type="CELLRANGE">
+                    <a:fld id="{1A2890E3-DB8D-42EF-A795-AD6CCA49346D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1274,7 +1274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{557D7F0B-A7C0-42A6-BC8E-162C2448132E}" type="CELLRANGE">
+                    <a:fld id="{60C949C5-1611-45F2-9E6F-2C8C53CD625F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1308,7 +1308,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C896FCF5-8317-4B30-A264-1DA549C3757E}" type="CELLRANGE">
+                    <a:fld id="{D4D68612-CCA0-49B6-9830-D0E34F1B886A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1342,7 +1342,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2179668-E49A-4508-8A10-858AD58F37E5}" type="CELLRANGE">
+                    <a:fld id="{4AB85D74-9107-4E2F-81B3-274F0CE7E10F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1376,7 +1376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE1C6796-9D29-41C1-A7CA-3B152D004ECC}" type="CELLRANGE">
+                    <a:fld id="{F3E7A3BB-8680-4CF0-B5B7-DD0074355218}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1410,7 +1410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DA1AD78-929D-42A7-9E6A-DDF9A5CFB514}" type="CELLRANGE">
+                    <a:fld id="{4F20CCEC-E509-4EE8-B518-955713B20A52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1444,7 +1444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6FFA838-46FE-4D5B-AA76-11BD277A4F90}" type="CELLRANGE">
+                    <a:fld id="{71F708FC-F909-456C-8DDE-FD0A169E049B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1478,7 +1478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6191FF0C-AB37-4673-B3BE-C09C761D079E}" type="CELLRANGE">
+                    <a:fld id="{7E114744-E1DA-4612-A54C-2D98B7858ACC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1512,7 +1512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26E7D6BB-CE4D-4BC8-BBD5-3F5239231C24}" type="CELLRANGE">
+                    <a:fld id="{CD0763E5-47F5-47BC-B51E-1A3FCF163A9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1546,7 +1546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1204938-0683-40DF-AF6A-B94140840537}" type="CELLRANGE">
+                    <a:fld id="{B1A7B38E-46C4-4080-A655-A8EE2F6D45FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2713,6 +2713,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3002,7 +3006,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3012,8 +3016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2143131-87F5-4AA4-9984-C0504AF0BF42}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="L9" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3086,7 +3090,7 @@
         <v>0.3</v>
       </c>
       <c r="G3">
-        <f>C3+D3-E3-F3</f>
+        <f t="shared" ref="G3:G14" si="0">C3+D3-E3-F3</f>
         <v>2.4900000000000002</v>
       </c>
       <c r="H3" s="1">
@@ -3097,7 +3101,7 @@
         <v>3210</v>
       </c>
       <c r="J3">
-        <f>G3*I3</f>
+        <f t="shared" ref="J3:J14" si="1">G3*I3</f>
         <v>7992.9000000000005</v>
       </c>
       <c r="K3">
@@ -3128,25 +3132,25 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G4">
-        <f>C4+D4-E4-F4</f>
+        <f t="shared" si="0"/>
         <v>2.3899999999999997</v>
       </c>
       <c r="H4" s="1">
         <v>0.214</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I14" si="0">H4*10000</f>
+        <f t="shared" ref="I4:I14" si="2">H4*10000</f>
         <v>2140</v>
       </c>
       <c r="J4">
-        <f>G4*I4</f>
+        <f t="shared" si="1"/>
         <v>5114.5999999999995</v>
       </c>
       <c r="K4">
         <v>9.7100000000000009</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L14" si="1">K4/J4</f>
+        <f t="shared" ref="L4:L14" si="3">K4/J4</f>
         <v>1.8984866851757716E-3</v>
       </c>
     </row>
@@ -3170,25 +3174,25 @@
         <v>0.26</v>
       </c>
       <c r="G5">
-        <f>C5+D5-E5-F5</f>
+        <f t="shared" si="0"/>
         <v>2.4400000000000004</v>
       </c>
       <c r="H5" s="1">
         <v>0.17899999999999999</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1790</v>
       </c>
       <c r="J5">
-        <f>G5*I5</f>
+        <f t="shared" si="1"/>
         <v>4367.6000000000004</v>
       </c>
       <c r="K5">
         <v>29</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.6398021796867839E-3</v>
       </c>
     </row>
@@ -3212,25 +3216,25 @@
         <v>0.24</v>
       </c>
       <c r="G6">
-        <f>C6+D6-E6-F6</f>
+        <f t="shared" si="0"/>
         <v>2.46</v>
       </c>
       <c r="H6" s="1">
         <v>0.17899999999999999</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1790</v>
       </c>
       <c r="J6">
-        <f>G6*I6</f>
+        <f t="shared" si="1"/>
         <v>4403.3999999999996</v>
       </c>
       <c r="K6">
         <v>51.71</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1743198437570969E-2</v>
       </c>
     </row>
@@ -3254,25 +3258,25 @@
         <v>0.3</v>
       </c>
       <c r="G7">
-        <f>C7+D7-E7-F7</f>
+        <f t="shared" si="0"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="H7" s="1">
         <v>0.107</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1070</v>
       </c>
       <c r="J7">
-        <f>G7*I7</f>
+        <f t="shared" si="1"/>
         <v>2664.3</v>
       </c>
       <c r="K7">
         <v>8.89</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.3367113313065347E-3</v>
       </c>
     </row>
@@ -3296,25 +3300,25 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G8">
-        <f>C8+D8-E8-F8</f>
+        <f t="shared" si="0"/>
         <v>2.3899999999999997</v>
       </c>
       <c r="H8" s="1">
         <v>0.107</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1070</v>
       </c>
       <c r="J8">
-        <f>G8*I8</f>
+        <f t="shared" si="1"/>
         <v>2557.2999999999997</v>
       </c>
       <c r="K8">
         <v>4</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5641496891252494E-3</v>
       </c>
     </row>
@@ -3338,25 +3342,25 @@
         <v>0.26</v>
       </c>
       <c r="G9">
-        <f>C9+D9-E9-F9</f>
+        <f t="shared" si="0"/>
         <v>2.4400000000000004</v>
       </c>
       <c r="H9" s="1">
         <v>0.107</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1070</v>
       </c>
       <c r="J9">
-        <f>G9*I9</f>
+        <f t="shared" si="1"/>
         <v>2610.8000000000006</v>
       </c>
       <c r="K9">
         <v>14</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.3623410448904538E-3</v>
       </c>
     </row>
@@ -3380,25 +3384,25 @@
         <v>0.24</v>
       </c>
       <c r="G10">
-        <f>C10+D10-E10-F10</f>
+        <f t="shared" si="0"/>
         <v>2.46</v>
       </c>
       <c r="H10" s="1">
         <v>0.32100000000000001</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3210</v>
       </c>
       <c r="J10">
-        <f>G10*I10</f>
+        <f t="shared" si="1"/>
         <v>7896.5999999999995</v>
       </c>
       <c r="K10">
         <v>26.44</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.3482764734189402E-3</v>
       </c>
     </row>
@@ -3422,25 +3426,25 @@
         <v>0.3</v>
       </c>
       <c r="G11">
-        <f>C11+D11-E11-F11</f>
+        <f t="shared" si="0"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="H11" s="1">
         <v>0.14299999999999999</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1429.9999999999998</v>
       </c>
       <c r="J11">
-        <f>G11*I11</f>
+        <f t="shared" si="1"/>
         <v>3560.7</v>
       </c>
       <c r="K11">
         <v>15</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.212654815064454E-3</v>
       </c>
     </row>
@@ -3464,25 +3468,25 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G12">
-        <f>C12+D12-E12-F12</f>
+        <f t="shared" si="0"/>
         <v>2.3899999999999997</v>
       </c>
       <c r="H12" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
       <c r="J12">
-        <f>G12*I12</f>
+        <f t="shared" si="1"/>
         <v>860.39999999999986</v>
       </c>
       <c r="K12">
         <v>5.8</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.7410506741050679E-3</v>
       </c>
     </row>
@@ -3506,25 +3510,25 @@
         <v>0.26</v>
       </c>
       <c r="G13">
-        <f>C13+D13-E13-F13</f>
+        <f t="shared" si="0"/>
         <v>2.4400000000000004</v>
       </c>
       <c r="H13" s="1">
         <v>0.17899999999999999</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1790</v>
       </c>
       <c r="J13">
-        <f>G13*I13</f>
+        <f t="shared" si="1"/>
         <v>4367.6000000000004</v>
       </c>
       <c r="K13">
         <v>17.100000000000001</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9151936990566901E-3</v>
       </c>
     </row>
@@ -3548,25 +3552,25 @@
         <v>0.24</v>
       </c>
       <c r="G14">
-        <f>C14+D14-E14-F14</f>
+        <f t="shared" si="0"/>
         <v>2.46</v>
       </c>
       <c r="H14" s="1">
         <v>0.25</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2500</v>
       </c>
       <c r="J14">
-        <f>G14*I14</f>
+        <f t="shared" si="1"/>
         <v>6150</v>
       </c>
       <c r="K14">
         <v>31.5</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1219512195121953E-3</v>
       </c>
     </row>
@@ -3633,7 +3637,7 @@
         <v>0.3</v>
       </c>
       <c r="G18">
-        <f>C18+D18-E18-F18</f>
+        <f t="shared" ref="G18:G26" si="4">C18+D18-E18-F18</f>
         <v>2.4900000000000002</v>
       </c>
       <c r="H18">
@@ -3675,25 +3679,25 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G19">
-        <f>C19+D19-E19-F19</f>
+        <f t="shared" si="4"/>
         <v>2.3899999999999997</v>
       </c>
       <c r="H19">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:I25" si="2">H19*10000</f>
+        <f t="shared" ref="I19:I25" si="5">H19*10000</f>
         <v>360</v>
       </c>
       <c r="J19">
-        <f t="shared" ref="J19:J26" si="3">G19*I19</f>
+        <f t="shared" ref="J19:J26" si="6">G19*I19</f>
         <v>860.39999999999986</v>
       </c>
       <c r="K19">
         <v>17.14</v>
       </c>
       <c r="L19">
-        <f t="shared" ref="L19:L26" si="4">K19/J19</f>
+        <f t="shared" ref="L19:L26" si="7">K19/J19</f>
         <v>1.9920966992096702E-2</v>
       </c>
     </row>
@@ -3717,25 +3721,25 @@
         <v>0.26</v>
       </c>
       <c r="G20">
-        <f>C20+D20-E20-F20</f>
+        <f t="shared" si="4"/>
         <v>2.4400000000000004</v>
       </c>
       <c r="H20">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>709.99999999999989</v>
       </c>
       <c r="J20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1732.4</v>
       </c>
       <c r="K20">
         <v>18.57</v>
       </c>
       <c r="L20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.0719233433387208E-2</v>
       </c>
     </row>
@@ -3759,25 +3763,25 @@
         <v>0.3</v>
       </c>
       <c r="G21">
-        <f>C21+D21-E21-F21</f>
+        <f t="shared" si="4"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="H21">
         <v>0.01</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>249.00000000000003</v>
       </c>
       <c r="K21">
         <v>1.22</v>
       </c>
       <c r="L21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.8995983935742962E-3</v>
       </c>
     </row>
@@ -3801,25 +3805,25 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G22">
-        <f>C22+D22-E22-F22</f>
+        <f t="shared" si="4"/>
         <v>2.3899999999999997</v>
       </c>
       <c r="H22">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>709.99999999999989</v>
       </c>
       <c r="J22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1696.8999999999994</v>
       </c>
       <c r="K22">
         <v>11.89</v>
       </c>
       <c r="L22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.0068949260416085E-3</v>
       </c>
     </row>
@@ -3843,25 +3847,25 @@
         <v>0.26</v>
       </c>
       <c r="G23">
-        <f>C23+D23-E23-F23</f>
+        <f t="shared" si="4"/>
         <v>2.4400000000000004</v>
       </c>
       <c r="H23">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>360</v>
       </c>
       <c r="J23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>878.40000000000009</v>
       </c>
       <c r="K23">
         <v>7.67</v>
       </c>
       <c r="L23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.7317850637522766E-3</v>
       </c>
     </row>
@@ -3885,25 +3889,25 @@
         <v>0.3</v>
       </c>
       <c r="G24">
-        <f>C24+D24-E24-F24</f>
+        <f t="shared" si="4"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="H24">
         <v>0.01</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>249.00000000000003</v>
       </c>
       <c r="K24">
         <v>1.5</v>
       </c>
       <c r="L24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6.0240963855421681E-3</v>
       </c>
     </row>
@@ -3927,25 +3931,25 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G25">
-        <f>C25+D25-E25-F25</f>
+        <f t="shared" si="4"/>
         <v>2.3899999999999997</v>
       </c>
       <c r="H25">
         <v>0.107</v>
       </c>
       <c r="I25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1070</v>
       </c>
       <c r="J25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2557.2999999999997</v>
       </c>
       <c r="K25">
         <v>8.5</v>
       </c>
       <c r="L25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.3238180893911552E-3</v>
       </c>
     </row>
@@ -3969,7 +3973,7 @@
         <v>0.26</v>
       </c>
       <c r="G26">
-        <f>C26+D26-E26-F26</f>
+        <f t="shared" si="4"/>
         <v>2.4400000000000004</v>
       </c>
       <c r="H26">
@@ -3980,14 +3984,14 @@
         <v>360</v>
       </c>
       <c r="J26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>878.40000000000009</v>
       </c>
       <c r="K26">
         <v>8.5</v>
       </c>
       <c r="L26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.6766848816029136E-3</v>
       </c>
     </row>

</xml_diff>